<commit_message>
Add stage 3 for B1-B2
</commit_message>
<xml_diff>
--- a/onurhizlan/evidence.xlsx
+++ b/onurhizlan/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\onurhizlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0k_onurhizlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADF1A25-BAB6-4B4B-B992-D12EE3FE2DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2278F3FB-9CDD-49DE-B6C7-7A8A9EE592A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="903" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
   <si>
     <t>TxHash</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>7BAA7642C2250AE32DB955C777C19B2C470A8D839B74BB4566C7E4314B5CDF30</t>
+  </si>
+  <si>
+    <t>0402D337EDA48FC520830DE8096AB6A429BCA96C1230FFE9A8D2AFD844BADF2A</t>
+  </si>
+  <si>
+    <t>A47AE2BDEC9179D0169FE5D8F5438D8FC6C1B9836791B5B55086CB127066F226</t>
+  </si>
+  <si>
+    <t>5F3CE35BE89900A27210E7179665E0F07D65979E60ED59E39E776679987C454A</t>
   </si>
 </sst>
 </file>
@@ -566,8 +578,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1223,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1225,12 +1239,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1245,7 +1259,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1259,12 +1275,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add round 4 / B5-B6-B7
</commit_message>
<xml_diff>
--- a/onurhizlan/evidence.xlsx
+++ b/onurhizlan/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0k_onurhizlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\-_0k_onurhizlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2278F3FB-9CDD-49DE-B6C7-7A8A9EE592A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4850A772-84AB-4EEF-BB51-CBA37DEDB7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="903" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="903" firstSheet="2" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,47 +38,27 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -176,13 +156,184 @@
   </si>
   <si>
     <t>5F3CE35BE89900A27210E7179665E0F07D65979E60ED59E39E776679987C454A</t>
+  </si>
+  <si>
+    <t>ibc/2B857045E99686EFDBC32BC89CD94F601F39B59E5EF9FB7A2EFDC3037D8E830B</t>
+  </si>
+  <si>
+    <t>hizlanA7</t>
+  </si>
+  <si>
+    <t>ibc/D9BD5AA9D5FD039AF03ADDE0A2142D743FCD62517E9EFF3FC8AA027ED87377C2</t>
+  </si>
+  <si>
+    <t>hizlanA8</t>
+  </si>
+  <si>
+    <t>ibc/A84CA7F4E13D7CE5E54D716A6B526D01FBE75535913D239ED1E6F17F25CAD23D</t>
+  </si>
+  <si>
+    <t>hizlanA9</t>
+  </si>
+  <si>
+    <t>ibc/C74D43B0A43CD41AD6046B18551145C0786CD8E602749E6BA2DFE495DE081753</t>
+  </si>
+  <si>
+    <t>hizlanA10</t>
+  </si>
+  <si>
+    <t>ibc/C7E8D1A34109E61B76886D272533915E6A68D44F210C99AE1CCBDB986C099092</t>
+  </si>
+  <si>
+    <t>hizlanA11</t>
+  </si>
+  <si>
+    <t>ibc/13CF7E33939781941E9DD89DF6E14309312C33D32491AE7436837DE1D866C184</t>
+  </si>
+  <si>
+    <t>hizlanA12</t>
+  </si>
+  <si>
+    <t>6BC47F30B14151FE0DD4475A9DAE17CF7DE2B7BA7818E6079110FA2B5793005F</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>C346671E6C0552003DE233DDCFBAF3AB3C394573AD7E4556AE02F05BFD46C767</t>
+  </si>
+  <si>
+    <t>AAEF972743612680F9D9A503FFDCD0A99B68F995B8DB930D4C916CBE10E5CA66</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>9E6B41D58702E411F2EEB0A2EC7B9454A9EDE03C3224041E0348BECB2F5FB19A</t>
+  </si>
+  <si>
+    <t>7F177815CA07E83931B31D6323498DF71AE119E3A0A32ADD33A054E893DA2D56</t>
+  </si>
+  <si>
+    <t>138B838EA6CA45C22AC8DC4B8B34AF270EC37E321D3BBFEFF3479A1AD8246BB7</t>
+  </si>
+  <si>
+    <t>9276E91DC84351C7597BCA37504B540723AAB74EAA060A98CA88D450724CA359</t>
+  </si>
+  <si>
+    <t>067BBA265F3B221F12855742B50ECA6A4B07DA16B1E51D22AAE5DE550098500A</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>76C4D9BBFD915F2A1BB4A3EF0AE82668BDEEBE31104CF7B38DDC3F78FB02A8C7</t>
+  </si>
+  <si>
+    <t>3829C3F3CD9E66BF3BABF616348F3D8601A0ECB678811AC6620EE170909315E4</t>
+  </si>
+  <si>
+    <t>4B22F8D9281B4BE84AFF9CFBA69877DFA4361EE481562595CDC84E7E2407D98C</t>
+  </si>
+  <si>
+    <t>26EFB960EC2436342B11363379E1E8441E1126DA9CC312390913E13188C2D556</t>
+  </si>
+  <si>
+    <t>488B2C0FCABF920EAEA4FE093D0567461B5C137821960E95F4E2C3409DFF95A7</t>
+  </si>
+  <si>
+    <t>8E3B9E963FBF66306E53455509EC224D8D57F33EB6952A96D390809EE19E50BA</t>
+  </si>
+  <si>
+    <t>C35DAC41CD0DBBB2EF4FEAFC70532E306DE12785812F1603FFC39B407F7BE38A</t>
+  </si>
+  <si>
+    <t>946580CCB41F68338C63F2B1CD360792B8DB06F79DE778D74F49980D1DD15C1D</t>
+  </si>
+  <si>
+    <t>8DBF3D840C4E08B7B0A98C3841816424C1B0E0A58AB404853E2B5DED5CCAC37A</t>
+  </si>
+  <si>
+    <t>AF2DDE635C7E9DF04C8FAA7AADD999A642E19C166D170D233D11B99BB936C666</t>
+  </si>
+  <si>
+    <t>41CB82056F3269AAE7D8E0F8FDF1F79212D6662462A6CB9A12E351F58F309741</t>
+  </si>
+  <si>
+    <t>E10F52A58CC75ECC28C481C266D8764BD5A4EFAE11CC7CD8BAC43E1597E6F715</t>
+  </si>
+  <si>
+    <t>88F62C64C07D1CA1564E09B8FBE613569CAC3713D22CAE180B9ECDA9D2C8FF5F</t>
+  </si>
+  <si>
+    <t>E6594AA5421A665ECD1AAEA12037C6430DC518DA504F482B67B742F491EF418B</t>
+  </si>
+  <si>
+    <t>FCB9E7316A021B58CD7AAE772503CFB6EA61C32AE18DD2ABB3E1D8EC4079E24C</t>
+  </si>
+  <si>
+    <t>BD7E5D9EDAF134E5474639D9D8D9905288ADF68E8816E46A7EB2653634F32224</t>
+  </si>
+  <si>
+    <t>B3860440F3138E9616B77808EC472DBEE289AF44E4CDBB9C0FBE591C5473F44B</t>
+  </si>
+  <si>
+    <t>DC05E91EAFB53B5DD7564592D8AE82111F60B9232AE64DEBF7057237F9762933</t>
+  </si>
+  <si>
+    <t>80E65C217B8863591FC78849E620186C4D74042BB2C0F01414F8807AE42232D7</t>
+  </si>
+  <si>
+    <t>58E115761C50A04B097BAB2DEB9EDEE04F9BFCFDD800FDCEBBF1D50E61CAB90C</t>
+  </si>
+  <si>
+    <t>524027C854D28A2C0B6349FEC3F2AF3A2DF4290E78FDECD2D472EFAF13CF35C0</t>
+  </si>
+  <si>
+    <t>41E8318ED895A653E250A40954733DF4FE40D935855FE041DFEB66827D5F2E81</t>
+  </si>
+  <si>
+    <t>5DC06A8030E6804D94370B614D2EEBEEE6AAD5663E77919ECEA4F5437D2416AF</t>
+  </si>
+  <si>
+    <t>8335A332DB82CB6A0A62DED2C2FC5DF0BBB7345A33D23072A768EE2625A58E2E</t>
+  </si>
+  <si>
+    <t>45B2CD6F9CA00C2D7A02ED934F78505955673E98A36410D9839C904C4E537DEE</t>
+  </si>
+  <si>
+    <t>5ECF97DC1423F5A7B149BF1BF153170DA8AACFC1E07E0DD535DB8D89F52AB8B2</t>
+  </si>
+  <si>
+    <t>97072A38DF44B450347D51697A4542423B1F11890CC0734ADA4DABF75CEC0387</t>
+  </si>
+  <si>
+    <t>6835F1B0EFB87B3BFD784D5F9E85DC5F1ECDEA996283C823683DA2860B63B121</t>
+  </si>
+  <si>
+    <t>BE1B4C8B55A2BADDF0C4E9C4D6C1F8E5E0B4CE8DE76FBF4FA73DB8CCA5281EFA</t>
+  </si>
+  <si>
+    <t>58E7EF76F10B6E155CFF6EF95535FA4B264211D1286E90AF05A53E6E2F571CD1</t>
+  </si>
+  <si>
+    <t>24B6BF4193A7405B4B8BA4D6032AC4E5BD523AFE26829970863FAAAFBE6F89CD</t>
+  </si>
+  <si>
+    <t>8B8A5F5E08417C83A3ADA36D1A5345ED18A572F6A76E8374A9BAAA4245253CB5</t>
+  </si>
+  <si>
+    <t>B0E4D7860BD4402D88317BF0181877A9C37173BD90D5C2522B1384863D18A0D7</t>
+  </si>
+  <si>
+    <t>84D5017E246B7AD328B829A06F9009200F6D8DCA76AB21752417A08BBC99C6C0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +352,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="4">
@@ -252,10 +424,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -271,9 +444,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{AC5B6FAB-F612-47BD-B408-6F2E7368525C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -596,54 +775,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -658,7 +837,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -668,33 +849,558 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -704,33 +1410,75 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -740,476 +1488,59 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1239,12 +1570,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1259,7 +1590,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1275,12 +1606,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1295,7 +1626,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1309,12 +1642,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1329,7 +1662,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1343,12 +1678,45 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5159A2-7543-4638-A77A-471FA4BB81A3}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1378,32 +1746,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1435,27 +1803,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1486,27 +1854,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1537,27 +1905,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1589,27 +1957,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1624,7 +1992,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1634,18 +2004,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1660,7 +2030,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1670,18 +2042,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>